<commit_message>
Add Temp file, fix xpath and fix linq
</commit_message>
<xml_diff>
--- a/MosExchange/Data/Config.xlsx
+++ b/MosExchange/Data/Config.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Value</t>
   </si>
@@ -67,6 +67,12 @@
   </si>
   <si>
     <t>Email</t>
+  </si>
+  <si>
+    <t>Result\</t>
+  </si>
+  <si>
+    <t>ResultFolderPath</t>
   </si>
 </sst>
 </file>
@@ -395,10 +401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -479,6 +485,14 @@
         <v>15</v>
       </c>
     </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>

</xml_diff>